<commit_message>
Added super exciting dissertation analyses.
I might have broken everything by trying to add a year column.
</commit_message>
<xml_diff>
--- a/Pub_Style.xlsx
+++ b/Pub_Style.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\craig_meta\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$478</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="628">
   <si>
     <t>Full Reference</t>
   </si>
@@ -1908,6 +1903,9 @@
   </si>
   <si>
     <t>YY01ACn</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2222,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2233,10 +2231,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C478"/>
+  <dimension ref="A1:D478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136:B137"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="D428" sqref="D428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2244,7 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -2256,8 +2254,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -2267,8 +2268,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -2279,7 +2283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -2290,7 +2294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -2301,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2312,7 +2316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>157</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>158</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -2367,7 +2371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>160</v>
       </c>
@@ -2378,7 +2382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -2389,7 +2393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>162</v>
       </c>
@@ -2400,7 +2404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2950,7 +2954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -2960,8 +2964,11 @@
       <c r="C65" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>214</v>
       </c>
@@ -2971,8 +2978,11 @@
       <c r="C66" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -2982,8 +2992,11 @@
       <c r="C67" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>216</v>
       </c>
@@ -2993,8 +3006,11 @@
       <c r="C68" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>217</v>
       </c>
@@ -3005,7 +3021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>218</v>
       </c>
@@ -3016,7 +3032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -3027,7 +3043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>220</v>
       </c>
@@ -3038,7 +3054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>221</v>
       </c>
@@ -3049,7 +3065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -3060,7 +3076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>223</v>
       </c>
@@ -3071,7 +3087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>224</v>
       </c>
@@ -3082,7 +3098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>225</v>
       </c>
@@ -3093,7 +3109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>226</v>
       </c>
@@ -3104,7 +3120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>227</v>
       </c>
@@ -3115,7 +3131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>228</v>
       </c>
@@ -3302,7 +3318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>245</v>
       </c>
@@ -3313,7 +3329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>246</v>
       </c>
@@ -3324,7 +3340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>247</v>
       </c>
@@ -3335,7 +3351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>248</v>
       </c>
@@ -3345,8 +3361,11 @@
       <c r="C100" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>249</v>
       </c>
@@ -3356,8 +3375,11 @@
       <c r="C101" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>250</v>
       </c>
@@ -3367,8 +3389,11 @@
       <c r="C102" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>251</v>
       </c>
@@ -3378,8 +3403,11 @@
       <c r="C103" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>252</v>
       </c>
@@ -3390,7 +3418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>253</v>
       </c>
@@ -3401,7 +3429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>254</v>
       </c>
@@ -3412,7 +3440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>255</v>
       </c>
@@ -3423,7 +3451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>256</v>
       </c>
@@ -3434,7 +3462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>257</v>
       </c>
@@ -3445,7 +3473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>258</v>
       </c>
@@ -3456,7 +3484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>259</v>
       </c>
@@ -3467,7 +3495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>260</v>
       </c>
@@ -3478,7 +3506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>261</v>
       </c>
@@ -3489,7 +3517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>262</v>
       </c>
@@ -3499,8 +3527,11 @@
       <c r="C114" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>263</v>
       </c>
@@ -3510,8 +3541,11 @@
       <c r="C115" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>264</v>
       </c>
@@ -3521,8 +3555,11 @@
       <c r="C116" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>265</v>
       </c>
@@ -3532,8 +3569,11 @@
       <c r="C117" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>266</v>
       </c>
@@ -3543,8 +3583,11 @@
       <c r="C118" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>267</v>
       </c>
@@ -3555,7 +3598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>268</v>
       </c>
@@ -3566,7 +3609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>269</v>
       </c>
@@ -3577,7 +3620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>270</v>
       </c>
@@ -3588,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>271</v>
       </c>
@@ -3599,7 +3642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>272</v>
       </c>
@@ -3610,7 +3653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>273</v>
       </c>
@@ -3621,7 +3664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>274</v>
       </c>
@@ -3632,7 +3675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>275</v>
       </c>
@@ -3643,7 +3686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>276</v>
       </c>
@@ -3654,7 +3697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>277</v>
       </c>
@@ -3665,7 +3708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>278</v>
       </c>
@@ -3676,7 +3719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>279</v>
       </c>
@@ -3687,7 +3730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>280</v>
       </c>
@@ -3698,7 +3741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>281</v>
       </c>
@@ -3709,7 +3752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>282</v>
       </c>
@@ -3720,7 +3763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>283</v>
       </c>
@@ -3731,7 +3774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>284</v>
       </c>
@@ -3742,7 +3785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>285</v>
       </c>
@@ -3753,7 +3796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>286</v>
       </c>
@@ -3763,8 +3806,11 @@
       <c r="C138" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>287</v>
       </c>
@@ -3774,8 +3820,11 @@
       <c r="C139" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>288</v>
       </c>
@@ -3785,8 +3834,11 @@
       <c r="C140" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>289</v>
       </c>
@@ -3796,8 +3848,11 @@
       <c r="C141" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>290</v>
       </c>
@@ -3808,7 +3863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>291</v>
       </c>
@@ -3819,7 +3874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>292</v>
       </c>
@@ -3830,7 +3885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>293</v>
       </c>
@@ -3841,7 +3896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>294</v>
       </c>
@@ -3852,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>295</v>
       </c>
@@ -3863,7 +3918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>296</v>
       </c>
@@ -3874,7 +3929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>297</v>
       </c>
@@ -3885,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>298</v>
       </c>
@@ -3896,7 +3951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>299</v>
       </c>
@@ -3907,7 +3962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>300</v>
       </c>
@@ -3918,7 +3973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>301</v>
       </c>
@@ -3929,7 +3984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>302</v>
       </c>
@@ -3940,7 +3995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>303</v>
       </c>
@@ -3951,7 +4006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>304</v>
       </c>
@@ -3961,8 +4016,11 @@
       <c r="C156" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>305</v>
       </c>
@@ -3973,7 +4031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>306</v>
       </c>
@@ -3984,7 +4042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>307</v>
       </c>
@@ -3995,7 +4053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>308</v>
       </c>
@@ -4006,7 +4064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>309</v>
       </c>
@@ -4017,7 +4075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>310</v>
       </c>
@@ -4028,7 +4086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>311</v>
       </c>
@@ -4039,7 +4097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>312</v>
       </c>
@@ -4050,7 +4108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>313</v>
       </c>
@@ -4061,7 +4119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>314</v>
       </c>
@@ -4072,7 +4130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>315</v>
       </c>
@@ -4083,7 +4141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>316</v>
       </c>
@@ -4093,8 +4151,11 @@
       <c r="C168" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>317</v>
       </c>
@@ -4104,8 +4165,11 @@
       <c r="C169" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>318</v>
       </c>
@@ -4116,7 +4180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>319</v>
       </c>
@@ -4127,7 +4191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>320</v>
       </c>
@@ -4138,7 +4202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>321</v>
       </c>
@@ -4149,7 +4213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>322</v>
       </c>
@@ -4160,7 +4224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>323</v>
       </c>
@@ -4171,7 +4235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>324</v>
       </c>
@@ -4182,7 +4246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>325</v>
       </c>
@@ -4193,7 +4257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>326</v>
       </c>
@@ -4203,8 +4267,11 @@
       <c r="C178" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>327</v>
       </c>
@@ -4214,8 +4281,11 @@
       <c r="C179" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>328</v>
       </c>
@@ -4226,7 +4296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>329</v>
       </c>
@@ -4237,7 +4307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>330</v>
       </c>
@@ -4248,7 +4318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>331</v>
       </c>
@@ -4259,7 +4329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>332</v>
       </c>
@@ -4270,7 +4340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>333</v>
       </c>
@@ -4281,7 +4351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>334</v>
       </c>
@@ -4292,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>335</v>
       </c>
@@ -4303,7 +4373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>336</v>
       </c>
@@ -4314,7 +4384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>337</v>
       </c>
@@ -4325,7 +4395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>338</v>
       </c>
@@ -4336,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>339</v>
       </c>
@@ -4347,7 +4417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>340</v>
       </c>
@@ -4534,7 +4604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -4545,7 +4615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>358</v>
       </c>
@@ -4556,7 +4626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>359</v>
       </c>
@@ -4567,7 +4637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>360</v>
       </c>
@@ -4578,7 +4648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>361</v>
       </c>
@@ -4589,7 +4659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>362</v>
       </c>
@@ -4600,7 +4670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>363</v>
       </c>
@@ -4611,7 +4681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>364</v>
       </c>
@@ -4622,7 +4692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>365</v>
       </c>
@@ -4633,7 +4703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>366</v>
       </c>
@@ -4644,7 +4714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>367</v>
       </c>
@@ -4655,7 +4725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>368</v>
       </c>
@@ -4666,7 +4736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>369</v>
       </c>
@@ -4676,8 +4746,11 @@
       <c r="C221" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D221">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>370</v>
       </c>
@@ -4687,8 +4760,11 @@
       <c r="C222" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D222">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>371</v>
       </c>
@@ -4699,7 +4775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>372</v>
       </c>
@@ -4886,7 +4962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>389</v>
       </c>
@@ -4897,7 +4973,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>390</v>
       </c>
@@ -4908,7 +4984,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>391</v>
       </c>
@@ -4919,7 +4995,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>392</v>
       </c>
@@ -4930,7 +5006,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>393</v>
       </c>
@@ -4941,7 +5017,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>394</v>
       </c>
@@ -4952,7 +5028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>395</v>
       </c>
@@ -4963,7 +5039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>396</v>
       </c>
@@ -4974,7 +5050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>397</v>
       </c>
@@ -4985,7 +5061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>398</v>
       </c>
@@ -4995,8 +5071,11 @@
       <c r="C250" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>399</v>
       </c>
@@ -5007,7 +5086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>400</v>
       </c>
@@ -5018,7 +5097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>401</v>
       </c>
@@ -5029,7 +5108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>402</v>
       </c>
@@ -5040,7 +5119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>403</v>
       </c>
@@ -5051,7 +5130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>404</v>
       </c>
@@ -5062,7 +5141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>405</v>
       </c>
@@ -5073,7 +5152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>406</v>
       </c>
@@ -5084,7 +5163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>407</v>
       </c>
@@ -5095,7 +5174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>408</v>
       </c>
@@ -5106,7 +5185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>409</v>
       </c>
@@ -5117,7 +5196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>410</v>
       </c>
@@ -5128,7 +5207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>411</v>
       </c>
@@ -5138,8 +5217,11 @@
       <c r="C263" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D263">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>412</v>
       </c>
@@ -5150,7 +5232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>413</v>
       </c>
@@ -5161,7 +5243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>414</v>
       </c>
@@ -5172,7 +5254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>415</v>
       </c>
@@ -5183,7 +5265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>416</v>
       </c>
@@ -5194,7 +5276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>417</v>
       </c>
@@ -5205,7 +5287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>418</v>
       </c>
@@ -5216,7 +5298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>419</v>
       </c>
@@ -5227,7 +5309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>420</v>
       </c>
@@ -5238,7 +5320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>421</v>
       </c>
@@ -5249,7 +5331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>422</v>
       </c>
@@ -5260,7 +5342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>423</v>
       </c>
@@ -5271,7 +5353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>424</v>
       </c>
@@ -5282,7 +5364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>425</v>
       </c>
@@ -5293,7 +5375,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>426</v>
       </c>
@@ -5304,7 +5386,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>427</v>
       </c>
@@ -5315,7 +5397,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>428</v>
       </c>
@@ -5326,7 +5408,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>429</v>
       </c>
@@ -5337,7 +5419,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>430</v>
       </c>
@@ -5348,7 +5430,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>431</v>
       </c>
@@ -5358,8 +5440,11 @@
       <c r="C283" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D283">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>432</v>
       </c>
@@ -5369,8 +5454,11 @@
       <c r="C284" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D284">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>433</v>
       </c>
@@ -5380,8 +5468,11 @@
       <c r="C285" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D285">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>434</v>
       </c>
@@ -5391,8 +5482,11 @@
       <c r="C286" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D286">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>435</v>
       </c>
@@ -5403,7 +5497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>436</v>
       </c>
@@ -5414,7 +5508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>437</v>
       </c>
@@ -5425,7 +5519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>438</v>
       </c>
@@ -5436,7 +5530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>439</v>
       </c>
@@ -5447,7 +5541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>440</v>
       </c>
@@ -5458,7 +5552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>441</v>
       </c>
@@ -5469,7 +5563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>442</v>
       </c>
@@ -5480,7 +5574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>443</v>
       </c>
@@ -5491,7 +5585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>444</v>
       </c>
@@ -5502,7 +5596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>445</v>
       </c>
@@ -5513,7 +5607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>446</v>
       </c>
@@ -5523,8 +5617,11 @@
       <c r="C298" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D298">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>447</v>
       </c>
@@ -5534,8 +5631,11 @@
       <c r="C299" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D299">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>448</v>
       </c>
@@ -5545,8 +5645,11 @@
       <c r="C300" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D300">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>449</v>
       </c>
@@ -5557,7 +5660,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>450</v>
       </c>
@@ -5568,7 +5671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>451</v>
       </c>
@@ -5579,7 +5682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>452</v>
       </c>
@@ -5766,7 +5869,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="321" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>469</v>
       </c>
@@ -5777,7 +5880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>470</v>
       </c>
@@ -5788,7 +5891,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="323" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>471</v>
       </c>
@@ -5799,7 +5902,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>472</v>
       </c>
@@ -5810,7 +5913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>473</v>
       </c>
@@ -5821,7 +5924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>474</v>
       </c>
@@ -5832,7 +5935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>475</v>
       </c>
@@ -5843,7 +5946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>476</v>
       </c>
@@ -5854,7 +5957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>477</v>
       </c>
@@ -5865,7 +5968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>478</v>
       </c>
@@ -5876,7 +5979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>479</v>
       </c>
@@ -5886,8 +5989,11 @@
       <c r="C331" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D331">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>480</v>
       </c>
@@ -5898,7 +6004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>481</v>
       </c>
@@ -5908,8 +6014,11 @@
       <c r="C333" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D333">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>482</v>
       </c>
@@ -5919,8 +6028,11 @@
       <c r="C334" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D334">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>483</v>
       </c>
@@ -5930,8 +6042,11 @@
       <c r="C335" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D335">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>484</v>
       </c>
@@ -6822,7 +6937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>565</v>
       </c>
@@ -6833,7 +6948,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="418" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>566</v>
       </c>
@@ -6844,7 +6959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>567</v>
       </c>
@@ -6855,7 +6970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>568</v>
       </c>
@@ -6866,7 +6981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="421" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>569</v>
       </c>
@@ -6877,7 +6992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>570</v>
       </c>
@@ -6888,7 +7003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="423" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>571</v>
       </c>
@@ -6899,7 +7014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>572</v>
       </c>
@@ -6910,7 +7025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="425" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>573</v>
       </c>
@@ -6921,7 +7036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="426" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>574</v>
       </c>
@@ -6932,7 +7047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>575</v>
       </c>
@@ -6942,8 +7057,11 @@
       <c r="C427" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="428" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D427">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>576</v>
       </c>
@@ -6953,8 +7071,11 @@
       <c r="C428" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="429" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D428">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>577</v>
       </c>
@@ -6964,8 +7085,11 @@
       <c r="C429" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="430" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D429">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>578</v>
       </c>
@@ -6976,7 +7100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="431" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>579</v>
       </c>
@@ -6987,7 +7111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="432" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>580</v>
       </c>
@@ -7506,10 +7630,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C478">
-    <filterColumn colId="0">
+    <filterColumn colId="2">
       <filters>
-        <filter val="CC06AB"/>
-        <filter val="CC06AC"/>
+        <filter val="Dissertation (unpub)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>